<commit_message>
graphics updates, need to set all project to hebrew
</commit_message>
<xml_diff>
--- a/storeitems.xlsx
+++ b/storeitems.xlsx
@@ -191,6 +191,24 @@
   </x:si>
   <x:si>
     <x:t>10/08/2024 20:14:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:41:49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:44:22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:44:24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:44:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:44:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/08/2024 11:44:28</x:t>
   </x:si>
   <x:si>
     <x:t>Hello Kitty Sticker</x:t>
@@ -1085,6 +1103,108 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
+    <x:row r="29" spans="1:14">
+      <x:c r="A29" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B29" s="0">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:14">
+      <x:c r="A30" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B30" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:14">
+      <x:c r="A31" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B31" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:14">
+      <x:c r="A32" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B32" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:14">
+      <x:c r="A33" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B33" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:14">
+      <x:c r="A34" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B34" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1114,13 +1234,13 @@
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B1" s="0">
         <x:v>20</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,13 +1322,13 @@
     </x:row>
     <x:row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B9" s="0">
         <x:v>125</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1224,13 +1344,13 @@
     </x:row>
     <x:row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A11" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B11" s="0">
         <x:v>99</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>